<commit_message>
Removed overriding credential asset names in Main.xaml, set UniFi credentials to Sam'sCreds in config.xlsx.
</commit_message>
<xml_diff>
--- a/Processes/FA_BillingMilestone/Data/Config.xlsx
+++ b/Processes/FA_BillingMilestone/Data/Config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_BillingMilestone\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\RpaUiPathProcess\Processes\FA_BillingMilestone\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D519EB-81E4-4C15-A37B-89CF903BB21B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33930" yWindow="2925" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33930" yWindow="2925" windowWidth="21600" windowHeight="11505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="150">
   <si>
     <t>Name</t>
   </si>
@@ -470,12 +469,15 @@
   </si>
   <si>
     <t>UQ_GM_REPT_MILESTONE_DUE</t>
+  </si>
+  <si>
+    <t>Sam'sCreds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -849,7 +851,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2003,10 +2005,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -3206,11 +3208,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3258,7 +3260,7 @@
         <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>149</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -4305,7 +4307,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BAA5A4A-F8AE-46C5-BCF2-977A2C0C3B13}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E117"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">

</xml_diff>

<commit_message>
ReportQuery.xaml: Saves report as CSV rather than XLS. Dispatch.xaml: Changed Read Range to Read CSV. InitAllSettings.xaml: Removed excel read range activities.
</commit_message>
<xml_diff>
--- a/Processes/FA_BillingMilestone/Data/Config.xlsx
+++ b/Processes/FA_BillingMilestone/Data/Config.xlsx
@@ -255,15 +255,9 @@
     <t>UpdateQueue</t>
   </si>
   <si>
-    <t>I found issues running the milestone report query: {0} at: {1}</t>
-  </si>
-  <si>
     <t>Mail Error</t>
   </si>
   <si>
-    <t>I couldn't send billing milestone approvals: {0} at: {1}</t>
-  </si>
-  <si>
     <t>Excel Error</t>
   </si>
   <si>
@@ -273,9 +267,6 @@
     <t>SystemError ExcelReport</t>
   </si>
   <si>
-    <t>I couldn't access {0} for getting the billing milestones:  {1} and {2} at: {3}</t>
-  </si>
-  <si>
     <t>SystemError DispatchMail</t>
   </si>
   <si>
@@ -336,9 +327,6 @@
     <t>2</t>
   </si>
   <si>
-    <t>I couldn't access my email as {0} due to: {1} at: {2}</t>
-  </si>
-  <si>
     <t>SystemError LoginUniFi</t>
   </si>
   <si>
@@ -441,9 +429,6 @@
     <t>Approval for {0:MMMM} has expired after {1} months</t>
   </si>
   <si>
-    <t>I couldn't handle the response for {0} due to: {1} at: {2}</t>
-  </si>
-  <si>
     <t>RuleException NotApproved</t>
   </si>
   <si>
@@ -472,6 +457,21 @@
   </si>
   <si>
     <t>Sam'sCreds</t>
+  </si>
+  <si>
+    <t>I couldn't access my email as {0} due to: {1} at {2}</t>
+  </si>
+  <si>
+    <t>I found issues running the milestone report query: {0} at {1}</t>
+  </si>
+  <si>
+    <t>I couldn't access {0} for getting the billing milestones:  {1} at {3}</t>
+  </si>
+  <si>
+    <t>I couldn't send billing milestone approvals: {0} at {1}</t>
+  </si>
+  <si>
+    <t>I couldn't handle the response for {0} due to: {1} at {2}</t>
   </si>
 </sst>
 </file>
@@ -944,7 +944,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -967,7 +967,7 @@
         <v>69</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2182,12 +2182,12 @@
         <v>56</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>57</v>
@@ -2202,32 +2202,32 @@
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B25" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3212,7 +3212,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3260,7 +3260,7 @@
         <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -4310,7 +4310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E117"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -4361,28 +4361,28 @@
         <v>47</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>52</v>
@@ -4391,28 +4391,28 @@
         <v>49</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>104</v>
+        <v>145</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>48</v>
@@ -4421,28 +4421,28 @@
         <v>50</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>44</v>
@@ -4451,13 +4451,13 @@
         <v>53</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>44</v>
@@ -4466,28 +4466,28 @@
         <v>53</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>48</v>
@@ -4496,67 +4496,67 @@
         <v>50</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>77</v>
+        <v>146</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>83</v>
+        <v>147</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>79</v>
+        <v>148</v>
       </c>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E16" s="5"/>
     </row>
@@ -4571,61 +4571,61 @@
     </row>
     <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E22" s="5"/>
     </row>
@@ -4643,81 +4643,81 @@
     </row>
     <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="5"/>

</xml_diff>

<commit_message>
Adjusted click selector for, define billing plan.
</commit_message>
<xml_diff>
--- a/Processes/FA_BillingMilestone/Data/Config.xlsx
+++ b/Processes/FA_BillingMilestone/Data/Config.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_BillingMilestone\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E733CA9-952B-4F68-9E9B-099DB41395C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -505,7 +499,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -626,7 +620,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -678,7 +672,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -872,18 +866,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -966,86 +960,86 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>35</v>
+      <c r="A10" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>90</v>
+      <c r="A11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
     </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2025,19 +2019,17 @@
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z1001"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2115,160 +2107,161 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>1000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6">
-        <v>1000</v>
+        <v>15000</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7">
-        <v>15000</v>
+        <v>60000</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <v>60000</v>
-      </c>
-      <c r="C8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:26" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.9</v>
-      </c>
-      <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>54</v>
+        <v>146</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B24" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B19" t="s">
         <v>151</v>
       </c>
     </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3234,24 +3227,17 @@
     <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3293,19 +3279,27 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>66</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
         <v>66</v>
@@ -3314,41 +3308,33 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>67</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-    </row>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4338,18 +4324,16 @@
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added missing config items back in from previous version.
</commit_message>
<xml_diff>
--- a/Processes/FA_BillingMilestone/Data/Config.xlsx
+++ b/Processes/FA_BillingMilestone/Data/Config.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="161">
   <si>
     <t>Name</t>
   </si>
@@ -494,13 +494,19 @@
   </si>
   <si>
     <t>The billing milestone wasn't updated because: {0}</t>
+  </si>
+  <si>
+    <t>\\nas02.storage.uq.edu.au\CA\ITS\Academic Services\RPA\TEST\FA_BillingMilestone\Bot Files</t>
+  </si>
+  <si>
+    <t>\\nas02.storage.uq.edu.au\CA\ITS\Academic Services\RPA\TEST\FA_BillingMilestone\Email Store</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -525,6 +531,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -543,10 +555,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -560,8 +573,10 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -866,7 +881,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -877,7 +892,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -972,6 +987,9 @@
       <c r="A7" t="s">
         <v>33</v>
       </c>
+      <c r="B7" s="11" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -994,6 +1012,9 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2020,6 +2041,10 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3237,7 +3262,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>